<commit_message>
Repair for getting Properties from Object Repository
</commit_message>
<xml_diff>
--- a/src/test/java/testing/dataEngine/TestSuite1.xlsx
+++ b/src/test/java/testing/dataEngine/TestSuite1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="155">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>AAAAAAAAA</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1271,10 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3776,7 +3773,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3860,7 +3857,7 @@
         <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3"/>
       <c r="G3" s="11" t="s">
@@ -3868,7 +3865,7 @@
       </c>
       <c r="H3" s="12">
         <f>COUNTIF(C2:C44,"Yes")</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>41</v>
@@ -3900,7 +3897,7 @@
         <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3"/>
       <c r="G4" s="11" t="s">
@@ -3908,7 +3905,7 @@
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(C3:C45,"No")</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>40</v>
@@ -3940,7 +3937,7 @@
         <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -3952,7 +3949,7 @@
         <v>108</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -3964,7 +3961,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -3976,7 +3973,7 @@
         <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -3988,7 +3985,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -4000,7 +3997,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3"/>
     </row>

</xml_diff>